<commit_message>
Lector ocular terminado, aplicacion terminada
</commit_message>
<xml_diff>
--- a/entrenamiento/resultados/Aproximacion1.xlsx
+++ b/entrenamiento/resultados/Aproximacion1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive - Universidade da Coruña\UDC4\TFG\ComunicELA-tfg\entrenamiento\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8583E087-2028-414F-A188-1FC30F5FE4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D3F876-A393-4E46-BEA7-B2D952536728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30030" yWindow="1185" windowWidth="21600" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Modelo</t>
   </si>
@@ -79,19 +79,10 @@
     <t>9-4</t>
   </si>
   <si>
-    <t>Ya que dieron resultados similares, se realizan las graficas de precisiones para ver si la sigmoide es la culpable de llevar los resultados al centro de la pantalla</t>
-  </si>
-  <si>
-    <t>Se descarta esta opcion porque las gráficas resultantes son similares y tienen la misma problemática</t>
-  </si>
-  <si>
-    <t>Tercera observacion sin sigmoide ya que se vio que lleva el objetivo al centro y esto podia reducir la precisión</t>
-  </si>
-  <si>
-    <t>Se escoge el modelo 9 con la sigmoide por tener mejores resultados para la de fusión</t>
-  </si>
-  <si>
     <t>Segundas observaciones con el 9 por ser el mejor con los datos transformados</t>
+  </si>
+  <si>
+    <t>Aproximación inicial</t>
   </si>
 </sst>
 </file>
@@ -463,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,259 +481,274 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.1236999999999999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0132E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.17676800000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.7462999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.3406E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0505E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.184501</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.7065000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.0754000000000002E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.1287E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.17194499999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4.4621000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.0916000000000001E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.1712E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.17225099999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.5879000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>2.0503126084804531E-2</v>
-      </c>
-      <c r="C3">
-        <v>8.3085258167586058E-3</v>
-      </c>
-      <c r="D3">
-        <v>0.17783504192318239</v>
-      </c>
-      <c r="E3">
-        <v>3.6863775652591441E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1.9897566922008988E-2</v>
-      </c>
-      <c r="C4">
-        <v>8.4453719963676049E-3</v>
-      </c>
-      <c r="D4">
-        <v>0.1748960626976831</v>
-      </c>
-      <c r="E4">
-        <v>3.8223706475104029E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1.869786928208279E-2</v>
-      </c>
-      <c r="C5">
-        <v>8.1449344514923482E-3</v>
-      </c>
-      <c r="D5">
-        <v>0.16851789451071189</v>
-      </c>
-      <c r="E5">
-        <v>3.8050531679603858E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>2.0137639809399841E-2</v>
-      </c>
-      <c r="C6">
-        <v>7.714058709805155E-3</v>
-      </c>
-      <c r="D6">
-        <v>0.17323139778205329</v>
-      </c>
-      <c r="E6">
-        <v>3.4264073455487022E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>2.7064216575984439E-2</v>
-      </c>
-      <c r="C7">
-        <v>1.1137036413294429E-2</v>
-      </c>
-      <c r="D7">
-        <v>0.20158318515334811</v>
-      </c>
-      <c r="E7">
-        <v>4.5816432387074481E-2</v>
+      <c r="B7" s="2">
+        <v>2.4812000000000001E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.2513E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.18707299999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5.0906E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1.6571279126219449E-2</v>
-      </c>
-      <c r="C8">
-        <v>7.9934027949463918E-3</v>
-      </c>
-      <c r="D8">
-        <v>0.1575507045856544</v>
-      </c>
-      <c r="E8">
-        <v>4.1097938182467431E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1.6892366237672311E-2</v>
-      </c>
-      <c r="C9">
-        <v>8.1717042659146741E-3</v>
-      </c>
-      <c r="D9">
-        <v>0.1589075627071517</v>
-      </c>
-      <c r="E9">
-        <v>4.1273450440952562E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>1.6479621052608959E-2</v>
-      </c>
-      <c r="C10">
-        <v>8.2642816274501943E-3</v>
-      </c>
-      <c r="D10">
-        <v>0.156414130117212</v>
-      </c>
-      <c r="E10">
-        <v>4.0202726255387448E-2</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>1.631193415793989E-2</v>
-      </c>
-      <c r="C11">
-        <v>7.2693549314782786E-3</v>
-      </c>
-      <c r="D11">
-        <v>0.15691132715770181</v>
-      </c>
-      <c r="E11">
-        <v>3.6545012178000637E-2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>1.7785279259883931E-2</v>
+        <v>2.0503126084804531E-2</v>
       </c>
       <c r="C12">
-        <v>9.1891219310871568E-3</v>
+        <v>8.3085258167586093E-3</v>
       </c>
       <c r="D12">
-        <v>0.16374498541866031</v>
+        <v>0.17783504192318239</v>
       </c>
       <c r="E12">
-        <v>4.3025506106193073E-2</v>
+        <v>3.6863775652591441E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1.9897566922008988E-2</v>
+      </c>
+      <c r="C13">
+        <v>8.4453719963676049E-3</v>
+      </c>
+      <c r="D13">
+        <v>0.1748960626976831</v>
+      </c>
+      <c r="E13">
+        <v>3.8223706475104029E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>1.869786928208279E-2</v>
+      </c>
+      <c r="C14">
+        <v>8.1449344514923482E-3</v>
+      </c>
+      <c r="D14">
+        <v>0.16851789451071189</v>
+      </c>
+      <c r="E14">
+        <v>3.8050531679603858E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>1.848489055410028E-2</v>
+        <v>2.0137639809399841E-2</v>
       </c>
       <c r="C15">
-        <v>7.4966390184464634E-3</v>
+        <v>7.714058709805155E-3</v>
       </c>
       <c r="D15">
-        <v>0.16948757927332611</v>
+        <v>0.17323139778205329</v>
       </c>
       <c r="E15">
-        <v>3.2330354349791132E-2</v>
+        <v>3.4264073455487022E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>1.73350499443976E-2</v>
+        <v>2.7064216575984439E-2</v>
       </c>
       <c r="C16">
-        <v>8.0260181891806011E-3</v>
+        <v>1.1137036413294429E-2</v>
       </c>
       <c r="D16">
-        <v>0.16131076972399441</v>
+        <v>0.20158318515334811</v>
       </c>
       <c r="E16">
-        <v>3.7795362004923047E-2</v>
+        <v>4.5816432387074481E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>2.062206539059324E-2</v>
+        <v>1.6571279126219449E-2</v>
       </c>
       <c r="C17">
-        <v>7.7016779662840811E-3</v>
+        <v>7.9934027949463918E-3</v>
       </c>
       <c r="D17">
-        <v>0.1756994375160762</v>
+        <v>0.1575507045856544</v>
       </c>
       <c r="E17">
-        <v>3.155273962821064E-2</v>
+        <v>4.1097938182467403E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>1.6892366237672311E-2</v>
+      </c>
+      <c r="C18">
+        <v>8.1717042659146741E-3</v>
+      </c>
+      <c r="D18">
+        <v>0.1589075627071517</v>
+      </c>
+      <c r="E18">
+        <v>4.1273450440952562E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>1.6479621052609E-2</v>
+      </c>
+      <c r="C19">
+        <v>8.2642816274501908E-3</v>
+      </c>
+      <c r="D19">
+        <v>0.156414130117212</v>
+      </c>
+      <c r="E19">
+        <v>4.02027262553874E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>1.6311934157939901E-2</v>
+      </c>
+      <c r="C20">
+        <v>7.2693549314782804E-3</v>
+      </c>
+      <c r="D20">
+        <v>0.15691132715770201</v>
+      </c>
+      <c r="E20">
+        <v>3.6545012178000602E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>45301</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.8205272000000002E-2</v>
-      </c>
-      <c r="C21" s="2">
-        <v>6.6849179999999998E-3</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.16617932899999999</v>
-      </c>
-      <c r="E21" s="2">
-        <v>3.1552498999999998E-2</v>
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>1.7785279259883931E-2</v>
+      </c>
+      <c r="C21">
+        <v>9.1891219310871568E-3</v>
+      </c>
+      <c r="D21">
+        <v>0.16374498541866031</v>
+      </c>
+      <c r="E21">
+        <v>4.3025506106193073E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -752,15 +758,71 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <v>1.848489055410028E-2</v>
+      </c>
+      <c r="C24">
+        <v>7.4966390184464634E-3</v>
+      </c>
+      <c r="D24">
+        <v>0.16948757927332611</v>
+      </c>
+      <c r="E24">
+        <v>3.2330354349791132E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>1.73350499443976E-2</v>
+      </c>
+      <c r="C25">
+        <v>8.0260181891806011E-3</v>
+      </c>
+      <c r="D25">
+        <v>0.16131076972399441</v>
+      </c>
+      <c r="E25">
+        <v>3.7795362004923047E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>2.062206539059324E-2</v>
+      </c>
+      <c r="C26">
+        <v>7.7016779662840811E-3</v>
+      </c>
+      <c r="D26">
+        <v>0.1756994375160762</v>
+      </c>
+      <c r="E26">
+        <v>3.155273962821064E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>